<commit_message>
Updates spells and created a pull spell
</commit_message>
<xml_diff>
--- a/Burn Down Charts/Lucian Burn Down Chart.xlsx
+++ b/Burn Down Charts/Lucian Burn Down Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\Wacky-Wizards\Burn Down Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{166CDAC8-3F1E-495E-B642-65D1C248DE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596202CA-001B-4440-A173-4D5D8F7E88FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Days Work Per Week</t>
   </si>
@@ -57,45 +57,6 @@
     <t>Completion Time in Days on the 16/10/23</t>
   </si>
   <si>
-    <t>Enemy Movement</t>
-  </si>
-  <si>
-    <t>Enemy Vision(dot product research)</t>
-  </si>
-  <si>
-    <t>Enemy Vision</t>
-  </si>
-  <si>
-    <t>Enemy Vision(dot product Test)</t>
-  </si>
-  <si>
-    <t>Enemy Vision(onOverlap)</t>
-  </si>
-  <si>
-    <t>Mantle(transform .z change)</t>
-  </si>
-  <si>
-    <t>Mantle(collision sphere)</t>
-  </si>
-  <si>
-    <t>Mantle(collision sphere, disabled)</t>
-  </si>
-  <si>
-    <t>Mantle Research</t>
-  </si>
-  <si>
-    <t>Mantle(checking if in air)</t>
-  </si>
-  <si>
-    <t>Mantle(checking in air research)</t>
-  </si>
-  <si>
-    <t>Mantle(testing)</t>
-  </si>
-  <si>
-    <t>Mantle/ climb up (removed)</t>
-  </si>
-  <si>
     <t>Research on local multiplayer</t>
   </si>
   <si>
@@ -172,6 +133,9 @@
   </si>
   <si>
     <t>Spells crashing game (no bueno)</t>
+  </si>
+  <si>
+    <t>Local Multiplayer</t>
   </si>
 </sst>
 </file>
@@ -394,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -408,16 +372,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -441,10 +401,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -510,7 +466,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BurnDownSrint2!$A$50</c:f>
+              <c:f>BurnDownSrint2!$A$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -524,7 +480,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BurnDownSrint2!$B$50:$F$50</c:f>
+              <c:f>BurnDownSrint2!$B$36:$F$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -558,7 +514,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>BurnDownSrint2!$A$51</c:f>
+              <c:f>BurnDownSrint2!$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -572,12 +528,12 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BurnDownSrint2!$B$51:$F$51</c:f>
+              <c:f>BurnDownSrint2!$B$37:$F$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.3999999999999968</c:v>
+                  <c:v>6.8999999999999977</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.3000000000000007</c:v>
@@ -1025,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,19 +1009,19 @@
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="16">
+      <c r="C1" s="14">
         <v>45222</v>
       </c>
-      <c r="D1" s="16">
+      <c r="D1" s="14">
         <v>45229</v>
       </c>
-      <c r="E1" s="16">
+      <c r="E1" s="14">
         <v>45236</v>
       </c>
-      <c r="F1" s="16">
+      <c r="F1" s="14">
         <v>45243</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -1078,732 +1034,536 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="25">
-        <v>0</v>
-      </c>
-      <c r="C2" s="25">
-        <v>0</v>
-      </c>
-      <c r="D2" s="25">
-        <v>0</v>
-      </c>
-      <c r="E2" s="25">
-        <v>0</v>
-      </c>
-      <c r="F2" s="25">
-        <v>0</v>
-      </c>
-      <c r="G2" s="26">
+    <row r="2" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="21">
+        <v>0</v>
+      </c>
+      <c r="C2" s="21">
+        <v>0</v>
+      </c>
+      <c r="D2" s="21">
+        <v>0</v>
+      </c>
+      <c r="E2" s="21">
+        <v>0</v>
+      </c>
+      <c r="F2" s="21">
+        <v>0</v>
+      </c>
+      <c r="G2" s="22">
         <v>2.5</v>
       </c>
-      <c r="H2" s="27">
+      <c r="H2" s="23">
         <v>4</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="24" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="C3" s="11">
-        <v>0</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
+        <v>8</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="C4" s="11">
-        <v>0</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="18"/>
+        <v>9</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="11">
+        <v>13</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="10">
         <v>0.3</v>
       </c>
-      <c r="C5" s="11">
-        <v>0</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="18"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="18"/>
-    </row>
-    <row r="7" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="19">
-        <v>0</v>
-      </c>
-      <c r="C7" s="19">
-        <v>0</v>
-      </c>
-      <c r="D7" s="19">
-        <v>0</v>
-      </c>
-      <c r="E7" s="19">
-        <v>0</v>
-      </c>
-      <c r="F7" s="19">
-        <v>0</v>
-      </c>
+      <c r="C6" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="C8" s="12">
-        <v>0</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="B8" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="C9" s="12">
-        <v>0</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+        <v>17</v>
+      </c>
+      <c r="B9" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="C10" s="12">
-        <v>0</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="C11" s="12">
-        <v>0</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="A11" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="17">
+        <v>0</v>
+      </c>
+      <c r="C11" s="17">
+        <v>0</v>
+      </c>
+      <c r="D11" s="17">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0</v>
+      </c>
+      <c r="F11" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="C12" s="12">
-        <v>0</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="A12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="C13" s="12">
-        <v>0</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+        <v>20</v>
+      </c>
+      <c r="B13" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="C13" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="C14" s="12">
-        <v>0</v>
-      </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+        <v>21</v>
+      </c>
+      <c r="B14" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="23">
-        <v>0</v>
-      </c>
-      <c r="C16" s="23">
-        <v>0</v>
-      </c>
-      <c r="D16" s="23">
-        <v>0</v>
-      </c>
-      <c r="E16" s="23">
-        <v>0</v>
-      </c>
-      <c r="F16" s="23">
-        <v>0</v>
-      </c>
+      <c r="A15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="C17" s="12">
-        <v>0</v>
-      </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="A17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="C18" s="12">
-        <v>0</v>
-      </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
+        <v>24</v>
+      </c>
+      <c r="B18" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="C18" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="C19" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="17">
+        <v>0</v>
+      </c>
+      <c r="C21" s="17">
+        <v>0</v>
+      </c>
+      <c r="D21" s="17">
+        <v>0</v>
+      </c>
+      <c r="E21" s="17">
+        <v>0</v>
+      </c>
+      <c r="F21" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="C22" s="11">
+        <v>0</v>
+      </c>
+      <c r="D22" s="11">
+        <v>0</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B25" s="10">
         <v>0.1</v>
       </c>
-      <c r="C19" s="12">
-        <v>0</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="C20" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="13">
-        <v>0.6</v>
-      </c>
-      <c r="C21" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="13">
+      <c r="C25" s="10">
         <v>0.1</v>
       </c>
-      <c r="C22" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="C23" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="19">
-        <v>0</v>
-      </c>
-      <c r="C25" s="19">
-        <v>0</v>
-      </c>
-      <c r="D25" s="19">
-        <v>0</v>
-      </c>
-      <c r="E25" s="19">
-        <v>0</v>
-      </c>
-      <c r="F25" s="19">
-        <v>0</v>
-      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="12">
-        <v>0.7</v>
-      </c>
-      <c r="C26" s="12">
-        <v>0.7</v>
-      </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+        <v>27</v>
+      </c>
+      <c r="B26" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="C26" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="C27" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="A27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="C27" s="11">
+        <v>0</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="C28" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="A28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="C28" s="11">
+        <v>0</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="12">
+        <v>30</v>
+      </c>
+      <c r="B29" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="C29" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="C30" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="10">
         <v>0.6</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C31" s="10">
         <v>0.6</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="12">
-        <v>0.6</v>
-      </c>
-      <c r="C30" s="12">
-        <v>0.6</v>
-      </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="12">
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="26">
         <v>0.2</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C32" s="26">
         <v>0.2</v>
       </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="C32" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="C33" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-    </row>
-    <row r="35" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="19">
-        <v>0</v>
-      </c>
-      <c r="C35" s="19">
-        <v>0</v>
-      </c>
-      <c r="D35" s="19">
-        <v>0</v>
-      </c>
-      <c r="E35" s="19">
-        <v>0</v>
-      </c>
-      <c r="F35" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+    </row>
+    <row r="35" spans="1:6" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="25"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="C36" s="13">
-        <v>0</v>
-      </c>
-      <c r="D36" s="13">
-        <v>0</v>
-      </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="C37" s="12">
-        <v>0</v>
-      </c>
-      <c r="D37" s="12">
-        <v>0</v>
-      </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="C39" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="C40" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="C41" s="13">
-        <v>0</v>
-      </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="C42" s="13">
-        <v>0</v>
-      </c>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="C43" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="C44" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="12">
-        <v>0.6</v>
-      </c>
-      <c r="C45" s="12">
-        <v>0.6</v>
-      </c>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="30">
-        <v>0.2</v>
-      </c>
-      <c r="C46" s="30">
-        <v>0.2</v>
-      </c>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="29"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="29"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="14">
+      <c r="B36" s="12">
         <f>(($G$2)*$H$2)</f>
         <v>10</v>
       </c>
-      <c r="C50" s="14">
-        <f>B50-($G$2)</f>
+      <c r="C36" s="12">
+        <f>B36-($G$2)</f>
         <v>7.5</v>
       </c>
-      <c r="D50" s="14">
-        <f>C50-($G$2)</f>
+      <c r="D36" s="12">
+        <f>C36-($G$2)</f>
         <v>5</v>
       </c>
-      <c r="E50" s="14">
-        <f>D50-($G$2)</f>
+      <c r="E36" s="12">
+        <f>D36-($G$2)</f>
         <v>2.5</v>
       </c>
-      <c r="F50" s="14">
-        <f>E50-($G$2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="9" t="s">
+      <c r="F36" s="12">
+        <f>E36-($G$2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="15">
-        <f t="shared" ref="B51:F51" si="0">SUM(B2:B45)</f>
-        <v>9.3999999999999968</v>
-      </c>
-      <c r="C51" s="15">
-        <f t="shared" si="0"/>
+      <c r="B37" s="13">
+        <f>SUM(B2:B31)</f>
+        <v>6.8999999999999977</v>
+      </c>
+      <c r="C37" s="13">
+        <f>SUM(C2:C31)</f>
         <v>5.3000000000000007</v>
       </c>
-      <c r="D51" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E51" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F51" s="15">
-        <f t="shared" si="0"/>
+      <c r="D37" s="13">
+        <f>SUM(D2:D31)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="13">
+        <f>SUM(E2:E31)</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="13">
+        <f>SUM(F2:F31)</f>
         <v>0</v>
       </c>
     </row>
@@ -1811,7 +1571,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C51" formulaRange="1"/>
+    <ignoredError sqref="C37" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>